<commit_message>
Update Sslb implementation (#599)
* Adjust Sslb implementation

* Update excel template
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sslb_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sslb_vorlage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse\SBIDER-2023-12\eclipse\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D964833-F1E9-4930-B7E2-9AFAF0E96F4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB67A110-184D-4688-A1BD-CD0ABE8D2F1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="23085" windowHeight="3705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sslb_Beispielbefüllung" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sslb_Beispielbefüllung!$A$1:$Y$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sslb_Beispielbefüllung!$A$1:$Z$7</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sslb_Beispielbefüllung!$A:$B,Sslb_Beispielbefüllung!$1:$5</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>A</t>
   </si>
@@ -154,10 +154,6 @@
   </si>
   <si>
     <t>Bezeichnung (Bedienung von)</t>
-  </si>
-  <si>
-    <t>Strecken-
-ziel</t>
   </si>
   <si>
     <t>W</t>
@@ -198,6 +194,19 @@
   <si>
     <t>Rückblock-
 wecker</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Regel-/Gegengleis</t>
+  </si>
+  <si>
+    <t>Streckenziel</t>
+  </si>
+  <si>
+    <t>Strecken-
+freimeldung</t>
   </si>
 </sst>
 </file>
@@ -618,7 +627,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -689,6 +698,18 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -707,12 +728,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -728,16 +743,16 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1091,44 +1106,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF7"/>
+  <dimension ref="A1:BG7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="10.35" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="10.35" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="7" style="4" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="7" style="4" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.42578125" style="4" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" style="4" customWidth="1"/>
-    <col min="15" max="16" width="7.42578125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="10.140625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="8.5703125" style="4" customWidth="1"/>
-    <col min="20" max="20" width="9" style="4" customWidth="1"/>
-    <col min="21" max="21" width="8.42578125" style="4" customWidth="1"/>
-    <col min="22" max="22" width="6.42578125" style="4" customWidth="1"/>
-    <col min="23" max="23" width="7" style="4" customWidth="1"/>
-    <col min="24" max="24" width="9.5703125" style="4" customWidth="1"/>
-    <col min="25" max="25" width="9.140625" style="4" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="4"/>
-    <col min="27" max="27" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="11.42578125" style="4"/>
+    <col min="5" max="5" width="7.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="7" style="4" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" style="4" customWidth="1"/>
+    <col min="11" max="12" width="7.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="5.42578125" style="4" customWidth="1"/>
+    <col min="16" max="17" width="7.42578125" style="4" customWidth="1"/>
+    <col min="18" max="18" width="10.140625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="8.7109375" style="4" customWidth="1"/>
+    <col min="20" max="20" width="7.42578125" style="4" customWidth="1"/>
+    <col min="21" max="21" width="8" style="4" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="6.42578125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="7" style="4" customWidth="1"/>
+    <col min="25" max="25" width="9.5703125" style="4" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" style="4" customWidth="1"/>
+    <col min="27" max="27" width="11.42578125" style="4"/>
+    <col min="28" max="28" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="10" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" s="10" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -1166,44 +1181,46 @@
       <c r="M1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="9" t="s">
         <v>14</v>
       </c>
       <c r="O1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="S1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="T1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="W1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="X1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
+      <c r="Z1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA1" s="9"/>
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
@@ -1235,190 +1252,197 @@
       <c r="BD1" s="4"/>
       <c r="BE1" s="4"/>
       <c r="BF1" s="4"/>
+      <c r="BG1" s="4"/>
     </row>
-    <row r="2" spans="1:58" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="33" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="24" t="s">
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
       <c r="Q2" s="39"/>
-      <c r="R2" s="32" t="s">
+      <c r="R2" s="40"/>
+      <c r="S2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="24" t="s">
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="25"/>
-      <c r="X2" s="11" t="s">
+      <c r="X2" s="29"/>
+      <c r="Y2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="Y2" s="12" t="s">
+      <c r="Z2" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:58" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="G3" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="37"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="42"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="30" t="s">
+      <c r="K3" s="42"/>
+      <c r="L3" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="L3" s="28" t="s">
+      <c r="N3" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" s="30" t="s">
+      <c r="R3" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="38"/>
+      <c r="U3" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="Q3" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="R3" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3" s="36"/>
-      <c r="T3" s="30" t="s">
+      <c r="V3" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="U3" s="28" t="s">
+      <c r="W3" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="V3" s="26" t="s">
+      <c r="X3" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="W3" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="X3" s="41" t="s">
+      <c r="Y3" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
     </row>
-    <row r="4" spans="1:58" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="31"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="33"/>
       <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="1" t="s">
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="T4" s="31"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="27"/>
-      <c r="W4" s="29"/>
-      <c r="X4" s="42"/>
-      <c r="Y4" s="7"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="33"/>
+      <c r="Y4" s="44"/>
+      <c r="Z4" s="7"/>
     </row>
-    <row r="5" spans="1:58" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:59" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="13"/>
       <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="14"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="16"/>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="13"/>
       <c r="T5" s="14"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="18"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="18"/>
     </row>
-    <row r="6" spans="1:58" ht="10.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" ht="10.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="20"/>
       <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="21"/>
       <c r="J6" s="21"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
@@ -1435,16 +1459,17 @@
       <c r="W6" s="20"/>
       <c r="X6" s="20"/>
       <c r="Y6" s="20"/>
+      <c r="Z6" s="20"/>
     </row>
-    <row r="7" spans="1:58" ht="10.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" ht="10.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="22"/>
       <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="23"/>
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
@@ -1461,32 +1486,34 @@
       <c r="W7" s="22"/>
       <c r="X7" s="22"/>
       <c r="Y7" s="22"/>
+      <c r="Z7" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="X3:X4"/>
+  <mergeCells count="24">
+    <mergeCell ref="Y3:Y4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="L3:L4"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:L2"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="R3:R4"/>
     <mergeCell ref="M3:M4"/>
-    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="U3:U4"/>
     <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:M2"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.19685039370078741" bottom="0.59055118110236227" header="0" footer="0"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>

</xml_diff>